<commit_message>
Ajout de fichier texte pour lister les ressource TODO: item commençant par le même nom
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,18 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Rune Age</t>
   </si>
   <si>
-    <t>12996</t>
+    <t>800000</t>
   </si>
   <si>
     <t>Rune Ga Pa</t>
-  </si>
-  <si>
-    <t>5759000</t>
   </si>
 </sst>
 </file>
@@ -467,7 +464,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>